<commit_message>
vignette ggsolvencyii and github README
</commit_message>
<xml_diff>
--- a/_data_helperfiles/preparingtables.xlsx
+++ b/_data_helperfiles/preparingtables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="6420" windowWidth="28800" windowHeight="6480" tabRatio="927" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="-15" yWindow="6420" windowWidth="28800" windowHeight="6480" tabRatio="927" firstSheet="10" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="struct_and_colors_sf16" sheetId="47" r:id="rId1"/>
@@ -32,7 +32,7 @@
     <sheet name="ex7_data" sheetId="35" r:id="rId23"/>
     <sheet name="ex7_plotdetails" sheetId="36" r:id="rId24"/>
   </sheets>
-  <calcPr calcId="145621" calcMode="manual"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -2713,12 +2713,14 @@
   </sheetPr>
   <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.5703125" style="54" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" style="54" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.5703125" style="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.5703125" bestFit="1" customWidth="1"/>
@@ -2744,10 +2746,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="75" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="54" t="s">
         <v>67</v>
       </c>
       <c r="C1" t="s">
@@ -2824,11 +2826,11 @@
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A2" s="15">
+      <c r="A2" s="54">
         <v>1</v>
       </c>
-      <c r="B2" s="15">
-        <v>1</v>
+      <c r="B2" s="54">
+        <v>2017</v>
       </c>
       <c r="C2" s="15">
         <v>230</v>
@@ -2917,7 +2919,7 @@
   <dimension ref="A1:AU5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AO12" sqref="AO12"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4202,14 +4204,14 @@
   </sheetPr>
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" style="54" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.5703125" style="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.5703125" bestFit="1" customWidth="1"/>
@@ -4227,7 +4229,7 @@
       <c r="A1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="54" t="s">
         <v>67</v>
       </c>
       <c r="C1" t="s">
@@ -4268,7 +4270,7 @@
       <c r="A2" s="19">
         <v>2</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="54">
         <v>2016</v>
       </c>
       <c r="C2" s="15">
@@ -4309,7 +4311,7 @@
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="54">
         <v>2015</v>
       </c>
       <c r="C3">
@@ -4348,7 +4350,7 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="54">
         <v>2017</v>
       </c>
       <c r="C4">
@@ -4448,7 +4450,7 @@
   <dimension ref="A1:AT4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AV30" sqref="AV30"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6594,12 +6596,12 @@
   <dimension ref="A1:BA2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B2" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="3.7109375" style="54" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="3.7109375" style="25" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="3.7109375" bestFit="1" customWidth="1"/>
@@ -6627,13 +6629,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" s="7" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="60" t="s">
         <v>67</v>
       </c>
       <c r="D1" s="7" t="s">
@@ -6789,10 +6791,10 @@
       </c>
     </row>
     <row r="2" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="54">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="54">
         <v>1</v>
       </c>
       <c r="D2">
@@ -7917,7 +7919,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8271,15 +8273,15 @@
   </sheetPr>
   <dimension ref="A1:AU3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" style="54" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="5.5703125" style="25" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4" style="22" bestFit="1" customWidth="1"/>
@@ -8317,7 +8319,7 @@
       <c r="B1" t="s">
         <v>165</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="54" t="s">
         <v>166</v>
       </c>
       <c r="D1" t="s">
@@ -8458,8 +8460,8 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>2</v>
+      <c r="C2" s="54">
+        <v>2017</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -8608,8 +8610,8 @@
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3">
-        <v>6</v>
+      <c r="C3" s="54">
+        <v>2022</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -9298,14 +9300,16 @@
   </sheetPr>
   <dimension ref="A1:AB11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D1:D1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" style="54" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="54" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.5703125" style="9" customWidth="1"/>
     <col min="6" max="7" width="8.5703125" customWidth="1"/>
     <col min="8" max="8" width="8.5703125" style="9" customWidth="1"/>
@@ -9322,7 +9326,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="75" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="54" t="s">
         <v>19</v>
       </c>
       <c r="B1" t="s">
@@ -9331,7 +9335,7 @@
       <c r="C1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="54" t="s">
         <v>22</v>
       </c>
       <c r="E1" s="8" t="s">
@@ -9405,22 +9409,19 @@
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A2" s="15">
+      <c r="A2" s="54">
         <v>1</v>
       </c>
-      <c r="B2" s="15">
-        <v>1</v>
+      <c r="B2" s="54">
+        <v>2016</v>
       </c>
       <c r="C2" s="15">
         <v>230</v>
       </c>
-      <c r="D2" s="15"/>
       <c r="E2" s="14">
-        <f>SUM(F2:H2)</f>
         <v>23</v>
       </c>
       <c r="F2" s="15">
-        <f>SUM(I2:L2)</f>
         <v>28</v>
       </c>
       <c r="G2" s="15">
@@ -9433,11 +9434,9 @@
         <v>-9</v>
       </c>
       <c r="J2" s="15">
-        <f>SUM(M2:S2)</f>
         <v>17</v>
       </c>
       <c r="K2" s="14">
-        <f t="shared" ref="K2:K11" si="0">SUM(T2:AA2)</f>
         <v>15</v>
       </c>
       <c r="L2" s="91">
@@ -9491,964 +9490,757 @@
       <c r="AB2" s="15"/>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A3" s="15">
-        <v>2</v>
-      </c>
-      <c r="B3" s="15">
-        <v>2</v>
+      <c r="A3" s="54">
+        <v>2</v>
+      </c>
+      <c r="B3" s="54">
+        <v>2017</v>
       </c>
       <c r="C3" s="15">
-        <f>+C2+4</f>
-        <v>234</v>
-      </c>
-      <c r="D3" s="15">
+        <v>233</v>
+      </c>
+      <c r="D3" s="54">
         <v>1</v>
       </c>
       <c r="E3" s="14">
-        <f t="shared" ref="E3:E11" ca="1" si="1">SUM(F3:H3)</f>
         <v>23.149926526465208</v>
       </c>
       <c r="F3" s="15">
-        <f ca="1">SUM(I3:L3)</f>
         <v>27.30838407992562</v>
       </c>
       <c r="G3" s="15">
         <v>5</v>
       </c>
       <c r="H3" s="94">
-        <f ca="1">+H$2*(_xlfn.NORM.INV(RAND(),1,0.07)*_xlfn.SUM(I3:O3)/_xlfn.SUM(I$2:O$2))</f>
         <v>-9.1584575534604067</v>
       </c>
       <c r="I3" s="89">
-        <f ca="1">+I$2*(_xlfn.NORM.INV(RAND(),1,0.07)*_xlfn.SUM(J3:P3)/_xlfn.SUM(J$2:P$2))</f>
         <v>-9.135998394490505</v>
       </c>
       <c r="J3" s="15">
-        <f t="shared" ref="J3:J11" ca="1" si="2">SUM(M3:S3)</f>
         <v>17.642394436184492</v>
       </c>
       <c r="K3" s="14">
-        <f t="shared" ca="1" si="0"/>
         <v>14.141988038231634</v>
       </c>
       <c r="L3" s="93">
-        <f t="shared" ref="L3:AA11" ca="1" si="3">ROUND(_xlfn.NORM.INV(RAND(),L$2,0.2*ABS(L$2)),2)</f>
         <v>4.66</v>
       </c>
       <c r="M3" s="89">
-        <f ca="1">+M$2*(_xlfn.NORM.INV(RAND(),1,0.07)*_xlfn.SUM(N3:T3)/_xlfn.SUM(N$2:T$2))</f>
         <v>-23.977605563815505</v>
       </c>
       <c r="N3" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>7.22</v>
       </c>
       <c r="O3" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>9.44</v>
       </c>
       <c r="P3" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>9.02</v>
       </c>
       <c r="Q3" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>5.14</v>
       </c>
       <c r="R3" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>5.73</v>
       </c>
       <c r="S3" s="93">
-        <f t="shared" ca="1" si="3"/>
         <v>5.07</v>
       </c>
       <c r="T3" s="89">
-        <f ca="1">+T$2*(_xlfn.NORM.INV(RAND(),1,0.07)*_xlfn.SUM(U3:AA3)/_xlfn.SUM(U$2:AA$2))</f>
         <v>-3.8780119617683675</v>
       </c>
       <c r="U3" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>1.31</v>
       </c>
       <c r="V3" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>1.99</v>
       </c>
       <c r="W3" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>3.16</v>
       </c>
       <c r="X3" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>3.8</v>
       </c>
       <c r="Y3" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>2.96</v>
       </c>
       <c r="Z3" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>2.89</v>
       </c>
       <c r="AA3" s="93">
-        <f ca="1">ROUND(_xlfn.NORM.INV(RAND(),AA$2,0.2*ABS(AA$2)),2)</f>
         <v>1.91</v>
       </c>
       <c r="AB3" s="15"/>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A4" s="15">
+      <c r="A4" s="54">
         <v>3</v>
       </c>
-      <c r="B4" s="15">
-        <v>3</v>
+      <c r="B4" s="54">
+        <v>2018</v>
       </c>
       <c r="C4" s="15">
-        <f>+C3+4</f>
         <v>238</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="54">
         <v>2</v>
       </c>
       <c r="E4" s="14">
-        <f t="shared" ca="1" si="1"/>
         <v>19.994608624208404</v>
       </c>
       <c r="F4" s="15">
-        <f t="shared" ref="F4:F11" ca="1" si="4">ROUND(_xlfn.NORM.INV(RAND(),F$2,0.2*ABS(F$2)),2)</f>
         <v>24.43</v>
       </c>
       <c r="G4" s="15">
         <v>5</v>
       </c>
       <c r="H4" s="94">
-        <f t="shared" ref="H4:H11" ca="1" si="5">+H$2*(_xlfn.NORM.INV(RAND(),1,0.07)*_xlfn.SUM(I4:O4)/_xlfn.SUM(I$2:O$2))</f>
         <v>-9.4353913757915944</v>
       </c>
       <c r="I4" s="89">
-        <f t="shared" ref="I4:I11" ca="1" si="6">+I$2*(_xlfn.NORM.INV(RAND(),1,0.07)*_xlfn.SUM(J4:P4)/_xlfn.SUM(J$2:P$2))</f>
         <v>-8.4025517451142502</v>
       </c>
       <c r="J4" s="15">
-        <f t="shared" ca="1" si="2"/>
         <v>14.56599732352014</v>
       </c>
       <c r="K4" s="14">
-        <f t="shared" ca="1" si="0"/>
         <v>15.777296867732911</v>
       </c>
       <c r="L4" s="93">
-        <f t="shared" ca="1" si="3"/>
         <v>4.1100000000000003</v>
       </c>
       <c r="M4" s="89">
-        <f t="shared" ref="M4:M11" ca="1" si="7">+M$2*(_xlfn.NORM.INV(RAND(),1,0.07)*_xlfn.SUM(N4:T4)/_xlfn.SUM(N$2:T$2))</f>
         <v>-16.104002676479858</v>
       </c>
       <c r="N4" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>6.63</v>
       </c>
       <c r="O4" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>4.08</v>
       </c>
       <c r="P4" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>6.71</v>
       </c>
       <c r="Q4" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>4.7699999999999996</v>
       </c>
       <c r="R4" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>3.93</v>
       </c>
       <c r="S4" s="93">
-        <f t="shared" ca="1" si="3"/>
         <v>4.55</v>
       </c>
       <c r="T4" s="89">
-        <f t="shared" ref="T4:T11" ca="1" si="8">+T$2*(_xlfn.NORM.INV(RAND(),1,0.07)*_xlfn.SUM(U4:AA4)/_xlfn.SUM(U$2:AA$2))</f>
         <v>-4.6127031322670877</v>
       </c>
       <c r="U4" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>1.27</v>
       </c>
       <c r="V4" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>2.1</v>
       </c>
       <c r="W4" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>3.14</v>
       </c>
       <c r="X4" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>6.03</v>
       </c>
       <c r="Y4" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>3.86</v>
       </c>
       <c r="Z4" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>1.94</v>
       </c>
       <c r="AA4" s="93">
-        <f t="shared" ca="1" si="3"/>
         <v>2.0499999999999998</v>
       </c>
       <c r="AB4" s="15"/>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A5" s="15">
+      <c r="A5" s="54">
         <v>4</v>
       </c>
-      <c r="B5" s="15">
-        <v>4</v>
+      <c r="B5" s="54">
+        <v>2019</v>
       </c>
       <c r="C5" s="15">
-        <f>+C4+4</f>
-        <v>242</v>
-      </c>
-      <c r="D5" s="15">
+        <v>243</v>
+      </c>
+      <c r="D5" s="54">
         <v>3</v>
       </c>
       <c r="E5" s="14">
-        <f t="shared" ca="1" si="1"/>
         <v>15.617731354988567</v>
       </c>
       <c r="F5" s="15">
-        <f t="shared" ca="1" si="4"/>
         <v>20.350000000000001</v>
       </c>
       <c r="G5" s="15">
         <v>5</v>
       </c>
       <c r="H5" s="94">
-        <f t="shared" ca="1" si="5"/>
         <v>-9.732268645011434</v>
       </c>
       <c r="I5" s="89">
-        <f t="shared" ca="1" si="6"/>
         <v>-7.8425117121816248</v>
       </c>
       <c r="J5" s="15">
-        <f t="shared" ca="1" si="2"/>
         <v>15.36936857962877</v>
       </c>
       <c r="K5" s="14">
-        <f t="shared" ca="1" si="0"/>
         <v>12.809102493057965</v>
       </c>
       <c r="L5" s="93">
-        <f t="shared" ca="1" si="3"/>
         <v>5.43</v>
       </c>
       <c r="M5" s="89">
-        <f t="shared" ca="1" si="7"/>
         <v>-20.090631420371231</v>
       </c>
       <c r="N5" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>8.39</v>
       </c>
       <c r="O5" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>6.29</v>
       </c>
       <c r="P5" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>5.5</v>
       </c>
       <c r="Q5" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>6.61</v>
       </c>
       <c r="R5" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>3.19</v>
       </c>
       <c r="S5" s="93">
-        <f t="shared" ca="1" si="3"/>
         <v>5.48</v>
       </c>
       <c r="T5" s="89">
-        <f t="shared" ca="1" si="8"/>
         <v>-3.0008975069420347</v>
       </c>
       <c r="U5" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>1.04</v>
       </c>
       <c r="V5" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>2.04</v>
       </c>
       <c r="W5" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>2.93</v>
       </c>
       <c r="X5" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>3.84</v>
       </c>
       <c r="Y5" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>2.34</v>
       </c>
       <c r="Z5" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>2.11</v>
       </c>
       <c r="AA5" s="93">
-        <f t="shared" ca="1" si="3"/>
         <v>1.51</v>
       </c>
       <c r="AB5" s="15"/>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A6" s="15">
+      <c r="A6" s="54">
         <v>5</v>
       </c>
-      <c r="B6" s="15">
-        <v>2</v>
+      <c r="B6" s="54">
+        <v>2017</v>
       </c>
       <c r="C6" s="15">
-        <f>+C2+1</f>
         <v>231</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="54">
         <v>1</v>
       </c>
       <c r="E6" s="14">
-        <f t="shared" ca="1" si="1"/>
         <v>19.605995252091482</v>
       </c>
       <c r="F6" s="15">
-        <f t="shared" ca="1" si="4"/>
         <v>21.29</v>
       </c>
       <c r="G6" s="15">
         <v>5</v>
       </c>
       <c r="H6" s="94">
-        <f t="shared" ca="1" si="5"/>
         <v>-6.684004747908519</v>
       </c>
       <c r="I6" s="89">
-        <f t="shared" ca="1" si="6"/>
         <v>-7.1846296545002639</v>
       </c>
       <c r="J6" s="15">
-        <f t="shared" ca="1" si="2"/>
         <v>15.419348782659444</v>
       </c>
       <c r="K6" s="14">
-        <f t="shared" ca="1" si="0"/>
         <v>13.183172314248182</v>
       </c>
       <c r="L6" s="93">
-        <f t="shared" ca="1" si="3"/>
         <v>4.2699999999999996</v>
       </c>
       <c r="M6" s="89">
-        <f t="shared" ca="1" si="7"/>
         <v>-21.750651217340554</v>
       </c>
       <c r="N6" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>7.18</v>
       </c>
       <c r="O6" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>5.42</v>
       </c>
       <c r="P6" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>5.8</v>
       </c>
       <c r="Q6" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>7.43</v>
       </c>
       <c r="R6" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>4.88</v>
       </c>
       <c r="S6" s="93">
-        <f t="shared" ca="1" si="3"/>
         <v>6.46</v>
       </c>
       <c r="T6" s="89">
-        <f t="shared" ca="1" si="8"/>
         <v>-3.686827685751819</v>
       </c>
       <c r="U6" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="V6" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>2.21</v>
       </c>
       <c r="W6" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>2.97</v>
       </c>
       <c r="X6" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>4.6900000000000004</v>
       </c>
       <c r="Y6" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>2.69</v>
       </c>
       <c r="Z6" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>2.39</v>
       </c>
       <c r="AA6" s="93">
-        <f t="shared" ca="1" si="3"/>
         <v>1.37</v>
       </c>
       <c r="AB6" s="15"/>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A7" s="15">
+      <c r="A7" s="54">
         <v>6</v>
       </c>
-      <c r="B7" s="15">
-        <v>3</v>
+      <c r="B7" s="54">
+        <v>2018</v>
       </c>
       <c r="C7" s="15">
-        <f>+C6+1</f>
         <v>232</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="54">
         <v>5</v>
       </c>
       <c r="E7" s="14">
-        <f t="shared" ca="1" si="1"/>
         <v>25.743364281293623</v>
       </c>
       <c r="F7" s="15">
-        <f t="shared" ca="1" si="4"/>
         <v>33.19</v>
       </c>
       <c r="G7" s="15">
         <v>5</v>
       </c>
       <c r="H7" s="94">
-        <f t="shared" ca="1" si="5"/>
         <v>-12.446635718706373</v>
       </c>
       <c r="I7" s="89">
-        <f t="shared" ca="1" si="6"/>
         <v>-10.961722332108064</v>
       </c>
       <c r="J7" s="15">
-        <f t="shared" ca="1" si="2"/>
         <v>21.584614925105491</v>
       </c>
       <c r="K7" s="14">
-        <f t="shared" ca="1" si="0"/>
         <v>17.296834075442753</v>
       </c>
       <c r="L7" s="93">
-        <f t="shared" ca="1" si="3"/>
         <v>5.99</v>
       </c>
       <c r="M7" s="89">
-        <f t="shared" ca="1" si="7"/>
         <v>-21.365385074894508</v>
       </c>
       <c r="N7" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>8.85</v>
       </c>
       <c r="O7" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>7.75</v>
       </c>
       <c r="P7" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>7.26</v>
       </c>
       <c r="Q7" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>8.32</v>
       </c>
       <c r="R7" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>4.72</v>
       </c>
       <c r="S7" s="93">
-        <f t="shared" ca="1" si="3"/>
         <v>6.05</v>
       </c>
       <c r="T7" s="89">
-        <f t="shared" ca="1" si="8"/>
         <v>-4.4831659245572482</v>
       </c>
       <c r="U7" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>1.1599999999999999</v>
       </c>
       <c r="V7" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>2.72</v>
       </c>
       <c r="W7" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>2.78</v>
       </c>
       <c r="X7" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>6.1</v>
       </c>
       <c r="Y7" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>4.32</v>
       </c>
       <c r="Z7" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>2.64</v>
       </c>
       <c r="AA7" s="93">
-        <f t="shared" ca="1" si="3"/>
         <v>2.06</v>
       </c>
       <c r="AB7" s="15"/>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A8" s="15">
+      <c r="A8" s="54">
         <v>7</v>
       </c>
-      <c r="B8" s="15">
-        <v>4</v>
+      <c r="B8" s="54">
+        <v>2019</v>
       </c>
       <c r="C8" s="15">
-        <f>+C7+1</f>
-        <v>233</v>
-      </c>
-      <c r="D8" s="15">
+        <v>232</v>
+      </c>
+      <c r="D8" s="54">
         <v>6</v>
       </c>
       <c r="E8" s="14">
-        <f t="shared" ca="1" si="1"/>
         <v>21.913415697015374</v>
       </c>
       <c r="F8" s="15">
-        <f t="shared" ca="1" si="4"/>
         <v>29.57</v>
       </c>
       <c r="G8" s="15">
         <v>5</v>
       </c>
       <c r="H8" s="94">
-        <f t="shared" ca="1" si="5"/>
         <v>-12.656584302984626</v>
       </c>
       <c r="I8" s="89">
-        <f t="shared" ca="1" si="6"/>
         <v>-9.2254163529275104</v>
       </c>
       <c r="J8" s="15">
-        <f t="shared" ca="1" si="2"/>
         <v>17.265390727836206</v>
       </c>
       <c r="K8" s="14">
-        <f t="shared" ca="1" si="0"/>
         <v>15.665464971097743</v>
       </c>
       <c r="L8" s="93">
-        <f t="shared" ca="1" si="3"/>
         <v>4.63</v>
       </c>
       <c r="M8" s="89">
-        <f t="shared" ca="1" si="7"/>
         <v>-13.794609272163791</v>
       </c>
       <c r="N8" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>5.57</v>
       </c>
       <c r="O8" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>5.43</v>
       </c>
       <c r="P8" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>5.71</v>
       </c>
       <c r="Q8" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>5.91</v>
       </c>
       <c r="R8" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>3.43</v>
       </c>
       <c r="S8" s="93">
-        <f t="shared" ca="1" si="3"/>
         <v>5.01</v>
       </c>
       <c r="T8" s="89">
-        <f t="shared" ca="1" si="8"/>
         <v>-4.2445350289022565</v>
       </c>
       <c r="U8" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="V8" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>2.4500000000000002</v>
       </c>
       <c r="W8" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>2.33</v>
       </c>
       <c r="X8" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>6.21</v>
       </c>
       <c r="Y8" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>4</v>
       </c>
       <c r="Z8" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>2.2599999999999998</v>
       </c>
       <c r="AA8" s="93">
-        <f t="shared" ca="1" si="3"/>
         <v>1.66</v>
       </c>
       <c r="AB8" s="15"/>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A9" s="15">
+      <c r="A9" s="54">
         <v>8</v>
       </c>
-      <c r="B9" s="15">
-        <v>2</v>
+      <c r="B9" s="54">
+        <v>2017</v>
       </c>
       <c r="C9" s="15">
-        <f>+C2-3</f>
         <v>227</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="54">
         <v>1</v>
       </c>
       <c r="E9" s="14">
-        <f t="shared" ca="1" si="1"/>
         <v>25.081685961650784</v>
       </c>
       <c r="F9" s="15">
-        <f t="shared" ca="1" si="4"/>
         <v>32.78</v>
       </c>
       <c r="G9" s="15">
         <v>5</v>
       </c>
       <c r="H9" s="94">
-        <f t="shared" ca="1" si="5"/>
         <v>-12.698314038349217</v>
       </c>
       <c r="I9" s="89">
-        <f t="shared" ca="1" si="6"/>
         <v>-9.2385032386626769</v>
       </c>
       <c r="J9" s="15">
-        <f t="shared" ca="1" si="2"/>
         <v>17.411609623645667</v>
       </c>
       <c r="K9" s="14">
-        <f t="shared" ca="1" si="0"/>
         <v>16.977486966021871</v>
       </c>
       <c r="L9" s="93">
-        <f t="shared" ca="1" si="3"/>
         <v>4.88</v>
       </c>
       <c r="M9" s="89">
-        <f t="shared" ca="1" si="7"/>
         <v>-14.918390376354331</v>
       </c>
       <c r="N9" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>7</v>
       </c>
       <c r="O9" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>5.5</v>
       </c>
       <c r="P9" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>5.9</v>
       </c>
       <c r="Q9" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>4.0599999999999996</v>
       </c>
       <c r="R9" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>3.67</v>
       </c>
       <c r="S9" s="93">
-        <f t="shared" ca="1" si="3"/>
         <v>6.2</v>
       </c>
       <c r="T9" s="89">
-        <f t="shared" ca="1" si="8"/>
         <v>-4.412513033978132</v>
       </c>
       <c r="U9" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>1.07</v>
       </c>
       <c r="V9" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>2.34</v>
       </c>
       <c r="W9" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>3.41</v>
       </c>
       <c r="X9" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>4.7300000000000004</v>
       </c>
       <c r="Y9" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>5.85</v>
       </c>
       <c r="Z9" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>2.5499999999999998</v>
       </c>
       <c r="AA9" s="93">
-        <f t="shared" ca="1" si="3"/>
         <v>1.44</v>
       </c>
       <c r="AB9" s="15"/>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A10" s="15">
+      <c r="A10" s="54">
         <v>9</v>
       </c>
-      <c r="B10" s="15">
-        <v>3</v>
+      <c r="B10" s="54">
+        <v>2018</v>
       </c>
       <c r="C10" s="15">
-        <f>+C9-2</f>
         <v>225</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="54">
         <v>8</v>
       </c>
       <c r="E10" s="14">
-        <f t="shared" ca="1" si="1"/>
         <v>22.430680753340773</v>
       </c>
       <c r="F10" s="15">
-        <f t="shared" ca="1" si="4"/>
         <v>26.28</v>
       </c>
       <c r="G10" s="15">
         <v>5</v>
       </c>
       <c r="H10" s="94">
-        <f t="shared" ca="1" si="5"/>
         <v>-8.8493192466592259</v>
       </c>
       <c r="I10" s="89">
-        <f t="shared" ca="1" si="6"/>
         <v>-9.3781450307394909</v>
       </c>
       <c r="J10" s="15">
-        <f t="shared" ca="1" si="2"/>
         <v>17.666611487669044</v>
       </c>
       <c r="K10" s="14">
-        <f t="shared" ca="1" si="0"/>
         <v>17.874622948386648</v>
       </c>
       <c r="L10" s="93">
-        <f t="shared" ca="1" si="3"/>
         <v>3.46</v>
       </c>
       <c r="M10" s="89">
-        <f t="shared" ca="1" si="7"/>
         <v>-19.903388512330956</v>
       </c>
       <c r="N10" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>5.65</v>
       </c>
       <c r="O10" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>6.28</v>
       </c>
       <c r="P10" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>5.67</v>
       </c>
       <c r="Q10" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>7.13</v>
       </c>
       <c r="R10" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>6.47</v>
       </c>
       <c r="S10" s="93">
-        <f t="shared" ca="1" si="3"/>
         <v>6.37</v>
       </c>
       <c r="T10" s="89">
-        <f t="shared" ca="1" si="8"/>
         <v>-4.9453770516133506</v>
       </c>
       <c r="U10" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>1.17</v>
       </c>
       <c r="V10" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>2.2200000000000002</v>
       </c>
       <c r="W10" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>2.86</v>
       </c>
       <c r="X10" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>6.92</v>
       </c>
       <c r="Y10" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>5.36</v>
       </c>
       <c r="Z10" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>2.2400000000000002</v>
       </c>
       <c r="AA10" s="93">
-        <f t="shared" ca="1" si="3"/>
         <v>2.0499999999999998</v>
       </c>
       <c r="AB10" s="15"/>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A11" s="15">
+      <c r="A11" s="54">
         <v>10</v>
       </c>
-      <c r="B11" s="15">
-        <v>4</v>
+      <c r="B11" s="54">
+        <v>2019</v>
       </c>
       <c r="C11" s="15">
-        <f>+C10+1</f>
         <v>226</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="54">
         <v>9</v>
       </c>
       <c r="E11" s="14">
-        <f t="shared" ca="1" si="1"/>
         <v>21.916074344891623</v>
       </c>
       <c r="F11" s="15">
-        <f t="shared" ca="1" si="4"/>
         <v>28.14</v>
       </c>
       <c r="G11" s="15">
         <v>5</v>
       </c>
       <c r="H11" s="94">
-        <f t="shared" ca="1" si="5"/>
         <v>-11.223925655108378</v>
       </c>
       <c r="I11" s="89">
-        <f t="shared" ca="1" si="6"/>
         <v>-10.838575434067343</v>
       </c>
       <c r="J11" s="15">
-        <f t="shared" ca="1" si="2"/>
         <v>19.815262287080252</v>
       </c>
       <c r="K11" s="14">
-        <f t="shared" ca="1" si="0"/>
         <v>15.148290177788503</v>
       </c>
       <c r="L11" s="93">
-        <f t="shared" ca="1" si="3"/>
         <v>4.7</v>
       </c>
       <c r="M11" s="89">
-        <f t="shared" ca="1" si="7"/>
         <v>-15.484737712919747</v>
       </c>
       <c r="N11" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>6.4</v>
       </c>
       <c r="O11" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>6.53</v>
       </c>
       <c r="P11" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>6.62</v>
       </c>
       <c r="Q11" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>6.36</v>
       </c>
       <c r="R11" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>3.38</v>
       </c>
       <c r="S11" s="93">
-        <f t="shared" ca="1" si="3"/>
         <v>6.01</v>
       </c>
       <c r="T11" s="89">
-        <f t="shared" ca="1" si="8"/>
         <v>-4.4017098222114956</v>
       </c>
       <c r="U11" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>0.88</v>
       </c>
       <c r="V11" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>1.94</v>
       </c>
       <c r="W11" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>4.6399999999999997</v>
       </c>
       <c r="X11" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>4.93</v>
       </c>
       <c r="Y11" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>4.2699999999999996</v>
       </c>
       <c r="Z11" s="89">
-        <f t="shared" ca="1" si="3"/>
         <v>1.65</v>
       </c>
       <c r="AA11" s="93">
-        <f t="shared" ca="1" si="3"/>
         <v>1.24</v>
       </c>
       <c r="AB11" s="15"/>

</xml_diff>